<commit_message>
Añadidos apellidos en los excel
</commit_message>
<xml_diff>
--- a/src/test/resources/testCandidatos.xlsx
+++ b/src/test/resources/testCandidatos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480000" yWindow="483090" windowWidth="15030" windowHeight="3690"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15030" windowHeight="3690"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -17,10 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Candidato</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Partido</t>
   </si>
@@ -53,6 +50,21 @@
   </si>
   <si>
     <t>Carlos</t>
+  </si>
+  <si>
+    <t>Apellido</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Alvarez</t>
+  </si>
+  <si>
+    <t>Baston</t>
+  </si>
+  <si>
+    <t>Cienfuegos</t>
   </si>
 </sst>
 </file>
@@ -391,57 +403,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C3:C5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
       </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>